<commit_message>
update scripts and some files
</commit_message>
<xml_diff>
--- a/datasets/raw_dataset.xlsx
+++ b/datasets/raw_dataset.xlsx
@@ -1198,7 +1198,7 @@
     <t xml:space="preserve">https://www.tamanmini.com/pesona_indonesia/museum-museum/museum-prangko-indonesia</t>
   </si>
   <si>
-    <t xml:space="preserve">dapat Potongan 10%</t>
+    <t xml:space="preserve">Dapat Potongan 10%</t>
   </si>
   <si>
     <t xml:space="preserve">46, 12, 24, 21.8, 15, 5.7</t>
@@ -1628,7 +1628,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1650,14 +1650,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1741,11 +1733,11 @@
   </sheetPr>
   <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q47" activeCellId="0" sqref="Q47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L46" activeCellId="0" sqref="L46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="59.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="117.43"/>
@@ -1884,7 +1876,7 @@
       <c r="E3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>35</v>
       </c>
       <c r="G3" s="0" t="s">
@@ -1972,10 +1964,10 @@
       <c r="E5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>53</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -2063,7 +2055,7 @@
       <c r="E7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="J7" s="0" t="s">
@@ -2110,7 +2102,7 @@
       <c r="E8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -3059,20 +3051,20 @@
       <c r="E31" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6" t="s">
+      <c r="G31" s="4"/>
+      <c r="H31" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J31" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K31" s="4" t="s">
         <v>263</v>
       </c>
       <c r="O31" s="4" t="s">
@@ -3113,10 +3105,10 @@
       <c r="I32" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="J32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K32" s="7" t="n">
+      <c r="K32" s="4" t="n">
         <v>0</v>
       </c>
       <c r="O32" s="4" t="s">
@@ -3148,10 +3140,10 @@
       <c r="E33" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="J33" s="4" t="s">
         <v>62</v>
       </c>
       <c r="K33" s="4" t="s">
@@ -3198,7 +3190,7 @@
       <c r="I34" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="J34" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K34" s="4" t="n">
@@ -3239,7 +3231,7 @@
       <c r="H35" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="J35" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K35" s="4" t="n">
@@ -3283,7 +3275,7 @@
       <c r="I36" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="J36" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K36" s="4" t="n">
@@ -3330,10 +3322,10 @@
       <c r="I37" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="J37" s="6" t="s">
+      <c r="J37" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="K37" s="7" t="s">
+      <c r="K37" s="4" t="s">
         <v>312</v>
       </c>
       <c r="O37" s="4" t="s">
@@ -3377,10 +3369,10 @@
       <c r="I38" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="J38" s="6" t="s">
+      <c r="J38" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="K38" s="7" t="s">
+      <c r="K38" s="4" t="s">
         <v>323</v>
       </c>
       <c r="O38" s="4" t="s">
@@ -3415,7 +3407,7 @@
       <c r="H39" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="J39" s="6" t="s">
+      <c r="J39" s="4" t="s">
         <v>330</v>
       </c>
       <c r="K39" s="4" t="s">
@@ -3471,10 +3463,10 @@
       <c r="I40" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="J40" s="6" t="s">
+      <c r="J40" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="K40" s="7" t="s">
+      <c r="K40" s="4" t="s">
         <v>343</v>
       </c>
       <c r="O40" s="4" t="s">
@@ -3518,25 +3510,25 @@
       <c r="I41" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="J41" s="6" t="s">
+      <c r="J41" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="K41" s="7" t="s">
+      <c r="K41" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="L41" s="7" t="s">
+      <c r="L41" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="M41" s="7" t="s">
+      <c r="M41" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="N41" s="7" t="s">
+      <c r="N41" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="O41" s="7" t="s">
+      <c r="O41" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P41" s="7" t="s">
+      <c r="P41" s="4" t="s">
         <v>357</v>
       </c>
       <c r="Q41" s="0" t="n">
@@ -3574,16 +3566,16 @@
       <c r="I42" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="J42" s="6" t="s">
+      <c r="J42" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K42" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O42" s="7" t="s">
+      <c r="O42" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="P42" s="7" t="s">
+      <c r="P42" s="4" t="s">
         <v>364</v>
       </c>
       <c r="Q42" s="0" t="n">
@@ -3609,7 +3601,7 @@
       <c r="E43" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="4" t="s">
         <v>368</v>
       </c>
       <c r="H43" s="0" t="s">
@@ -3618,16 +3610,16 @@
       <c r="I43" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="J43" s="6" t="s">
+      <c r="J43" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K43" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O43" s="7" t="s">
+      <c r="O43" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="P43" s="7" t="s">
+      <c r="P43" s="4" t="s">
         <v>371</v>
       </c>
       <c r="Q43" s="0" t="n">
@@ -3662,25 +3654,25 @@
       <c r="I44" s="0" t="s">
         <v>377</v>
       </c>
-      <c r="J44" s="6" t="s">
+      <c r="J44" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="K44" s="7" t="s">
+      <c r="K44" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="L44" s="7" t="s">
+      <c r="L44" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="M44" s="7" t="s">
+      <c r="M44" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="N44" s="7" t="s">
+      <c r="N44" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="O44" s="7" t="s">
+      <c r="O44" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="P44" s="7" t="s">
+      <c r="P44" s="4" t="s">
         <v>381</v>
       </c>
       <c r="Q44" s="0" t="n">
@@ -3706,7 +3698,7 @@
       <c r="E45" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="4" t="s">
         <v>386</v>
       </c>
       <c r="G45" s="0" t="s">
@@ -3715,16 +3707,16 @@
       <c r="H45" s="0" t="s">
         <v>387</v>
       </c>
-      <c r="J45" s="6" t="s">
+      <c r="J45" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K45" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O45" s="7" t="s">
+      <c r="O45" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P45" s="7" t="s">
+      <c r="P45" s="4" t="s">
         <v>388</v>
       </c>
       <c r="Q45" s="0" t="n">
@@ -3750,7 +3742,7 @@
       <c r="F46" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="J46" s="6" t="s">
+      <c r="J46" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K46" s="4" t="n">
@@ -3762,10 +3754,10 @@
       <c r="M46" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="O46" s="7" t="s">
+      <c r="O46" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="P46" s="7" t="s">
+      <c r="P46" s="4" t="s">
         <v>393</v>
       </c>
       <c r="Q46" s="0" t="n">
@@ -3797,25 +3789,25 @@
       <c r="I47" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="J47" s="6" t="s">
+      <c r="J47" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="K47" s="7" t="s">
+      <c r="K47" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="L47" s="7" t="s">
+      <c r="L47" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="M47" s="7" t="s">
+      <c r="M47" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N47" s="7" t="s">
+      <c r="N47" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="O47" s="7" t="s">
+      <c r="O47" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="P47" s="7" t="s">
+      <c r="P47" s="4" t="s">
         <v>399</v>
       </c>
       <c r="Q47" s="0" t="n">
@@ -3844,16 +3836,16 @@
       <c r="F48" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="J48" s="6" t="s">
+      <c r="J48" s="4" t="s">
         <v>404</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="O48" s="7" t="s">
+      <c r="O48" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="P48" s="7" t="s">
+      <c r="P48" s="4" t="s">
         <v>407</v>
       </c>
       <c r="Q48" s="0" t="n">
@@ -3879,16 +3871,16 @@
       <c r="E49" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="J49" s="6" t="s">
+      <c r="J49" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K49" s="4" t="n">
         <v>10000</v>
       </c>
-      <c r="O49" s="7" t="s">
+      <c r="O49" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P49" s="7" t="s">
+      <c r="P49" s="4" t="s">
         <v>411</v>
       </c>
       <c r="Q49" s="0" t="n">
@@ -3920,16 +3912,16 @@
       <c r="G50" s="0" t="s">
         <v>417</v>
       </c>
-      <c r="J50" s="6" t="s">
+      <c r="J50" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K50" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O50" s="7" t="s">
+      <c r="O50" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="P50" s="7" t="s">
+      <c r="P50" s="4" t="s">
         <v>419</v>
       </c>
       <c r="Q50" s="0" t="n">
@@ -3952,16 +3944,16 @@
       <c r="D51" s="0" t="s">
         <v>422</v>
       </c>
-      <c r="J51" s="6" t="s">
+      <c r="J51" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K51" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O51" s="7" t="s">
+      <c r="O51" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="P51" s="7" t="s">
+      <c r="P51" s="4" t="s">
         <v>424</v>
       </c>
       <c r="Q51" s="0" t="n">
@@ -3993,16 +3985,16 @@
       <c r="I52" s="0" t="s">
         <v>429</v>
       </c>
-      <c r="J52" s="6" t="s">
+      <c r="J52" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="K52" s="7" t="s">
+      <c r="K52" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="O52" s="7" t="s">
+      <c r="O52" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="P52" s="7" t="s">
+      <c r="P52" s="4" t="s">
         <v>432</v>
       </c>
       <c r="Q52" s="0" t="n">
@@ -4025,16 +4017,16 @@
       <c r="D53" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="J53" s="6" t="s">
+      <c r="J53" s="4" t="s">
         <v>245</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="O53" s="7" t="s">
+      <c r="O53" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="P53" s="7" t="s">
+      <c r="P53" s="4" t="s">
         <v>437</v>
       </c>
       <c r="Q53" s="0" t="n">
@@ -4069,25 +4061,25 @@
       <c r="I54" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="J54" s="6" t="s">
+      <c r="J54" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="K54" s="7" t="s">
+      <c r="K54" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="L54" s="7" t="s">
+      <c r="L54" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="M54" s="7" t="s">
+      <c r="M54" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N54" s="7" t="s">
+      <c r="N54" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="O54" s="7" t="s">
+      <c r="O54" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="P54" s="7" t="s">
+      <c r="P54" s="4" t="s">
         <v>448</v>
       </c>
       <c r="Q54" s="0" t="n">
@@ -4110,22 +4102,22 @@
       <c r="D55" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="E55" s="4" t="s">
         <v>451</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="J55" s="6" t="s">
+      <c r="J55" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K55" s="4" t="n">
         <v>25000</v>
       </c>
-      <c r="O55" s="7" t="s">
+      <c r="O55" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="P55" s="7" t="s">
+      <c r="P55" s="4" t="s">
         <v>453</v>
       </c>
       <c r="Q55" s="0" t="n">
@@ -4163,25 +4155,25 @@
       <c r="I56" s="0" t="s">
         <v>460</v>
       </c>
-      <c r="J56" s="6" t="s">
+      <c r="J56" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K56" s="7" t="s">
+      <c r="K56" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="L56" s="7" t="s">
+      <c r="L56" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="M56" s="7" t="s">
+      <c r="M56" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N56" s="7" t="s">
+      <c r="N56" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="O56" s="7" t="s">
+      <c r="O56" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="P56" s="7" t="s">
+      <c r="P56" s="4" t="s">
         <v>461</v>
       </c>
       <c r="Q56" s="0" t="n">
@@ -4213,25 +4205,25 @@
       <c r="I57" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="J57" s="6" t="s">
+      <c r="J57" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="K57" s="7" t="s">
+      <c r="K57" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="L57" s="7" t="s">
+      <c r="L57" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="M57" s="7" t="s">
+      <c r="M57" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N57" s="7" t="s">
+      <c r="N57" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="O57" s="7" t="s">
+      <c r="O57" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="P57" s="7" t="s">
+      <c r="P57" s="4" t="s">
         <v>469</v>
       </c>
       <c r="Q57" s="0" t="n">
@@ -4260,16 +4252,16 @@
       <c r="F58" s="0" t="s">
         <v>473</v>
       </c>
-      <c r="J58" s="6" t="s">
+      <c r="J58" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K58" s="4" t="n">
         <v>5000</v>
       </c>
-      <c r="O58" s="7" t="s">
+      <c r="O58" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="P58" s="7" t="s">
+      <c r="P58" s="4" t="s">
         <v>475</v>
       </c>
       <c r="Q58" s="0" t="n">
@@ -4304,16 +4296,16 @@
       <c r="I59" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="J59" s="6" t="s">
+      <c r="J59" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K59" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="O59" s="7" t="s">
+      <c r="O59" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="P59" s="7" t="s">
+      <c r="P59" s="4" t="s">
         <v>483</v>
       </c>
       <c r="Q59" s="0" t="n">
@@ -4339,22 +4331,22 @@
       <c r="E60" s="5" t="s">
         <v>486</v>
       </c>
-      <c r="F60" s="6" t="s">
+      <c r="F60" s="4" t="s">
         <v>487</v>
       </c>
       <c r="H60" s="0" t="s">
         <v>488</v>
       </c>
-      <c r="J60" s="6" t="s">
+      <c r="J60" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="K60" s="7" t="s">
+      <c r="K60" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="O60" s="7" t="s">
+      <c r="O60" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P60" s="7" t="s">
+      <c r="P60" s="4" t="s">
         <v>491</v>
       </c>
       <c r="Q60" s="0" t="n">
@@ -4383,16 +4375,16 @@
       <c r="H61" s="0" t="s">
         <v>496</v>
       </c>
-      <c r="J61" s="6" t="s">
+      <c r="J61" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="K61" s="7" t="s">
+      <c r="K61" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="O61" s="7" t="s">
+      <c r="O61" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="P61" s="7" t="s">
+      <c r="P61" s="4" t="s">
         <v>499</v>
       </c>
       <c r="Q61" s="0" t="n">
@@ -4430,16 +4422,16 @@
       <c r="I62" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="J62" s="6" t="s">
+      <c r="J62" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K62" s="4" t="n">
         <v>16500</v>
       </c>
-      <c r="O62" s="7" t="s">
+      <c r="O62" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P62" s="7" t="s">
+      <c r="P62" s="4" t="s">
         <v>506</v>
       </c>
       <c r="Q62" s="0" t="n">

</xml_diff>

<commit_message>
new datasets for entities & relations
</commit_message>
<xml_diff>
--- a/datasets/raw_dataset.xlsx
+++ b/datasets/raw_dataset.xlsx
@@ -1733,8 +1733,8 @@
   </sheetPr>
   <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L46" activeCellId="0" sqref="L46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N46" activeCellId="0" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1753,7 +1753,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="53.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="27.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="29.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="29.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.28"/>
@@ -3753,6 +3753,9 @@
       </c>
       <c r="M46" s="0" t="s">
         <v>143</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <v>4500</v>
       </c>
       <c r="O46" s="4" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
fix some typos in datasets
</commit_message>
<xml_diff>
--- a/datasets/raw_dataset.xlsx
+++ b/datasets/raw_dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="568">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">art1_newmuseum</t>
   </si>
   <si>
-    <t xml:space="preserve">Wisatawan Mancanegara, Umum, Pelajar, Anak – Anak</t>
+    <t xml:space="preserve">Wisatawan Mancanegara, Umum, Pelajar, Anak - Anak</t>
   </si>
   <si>
     <t xml:space="preserve">125000, 100000, 75000, 0</t>
@@ -1345,12 +1345,6 @@
     <t xml:space="preserve">MuseumNasProk</t>
   </si>
   <si>
-    <t xml:space="preserve">Dewasa, Anak – Anak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dewasa, Anak – Anak, Wisatawan Mancanegara</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rombongan (min. 20 Orang)</t>
   </si>
   <si>
@@ -1423,7 +1417,7 @@
     <t xml:space="preserve">https://www.tamanmini.com/pesona_indonesia/museum-museum/museum-purna-bhakti-pertiwi</t>
   </si>
   <si>
-    <t xml:space="preserve">Anak – Anak, Dewasa</t>
+    <t xml:space="preserve">Anak - Anak, Dewasa</t>
   </si>
   <si>
     <t xml:space="preserve">3000, 5000</t>
@@ -1949,10 +1943,10 @@
   </sheetPr>
   <dimension ref="A1:AE62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="AC41" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
-      <selection pane="topRight" activeCell="AC60" activeCellId="0" sqref="AC60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="X25" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topRight" activeCell="Y44" activeCellId="0" sqref="Y44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4594,16 +4588,16 @@
         <v>440</v>
       </c>
       <c r="W44" s="11" t="s">
-        <v>441</v>
+        <v>99</v>
       </c>
       <c r="X44" s="9" t="s">
         <v>158</v>
       </c>
       <c r="Y44" s="9" t="s">
-        <v>442</v>
+        <v>188</v>
       </c>
       <c r="Z44" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="AA44" s="9" t="s">
         <v>190</v>
@@ -4612,7 +4606,7 @@
         <v>126</v>
       </c>
       <c r="AC44" s="11" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="AD44" s="0" t="n">
         <v>-6.20037495844248</v>
@@ -4623,7 +4617,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>64</v>
@@ -4638,25 +4632,25 @@
         <v>53</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="P45" s="0" t="s">
         <v>131</v>
       </c>
       <c r="Q45" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="S45" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="R45" s="1" t="s">
+      <c r="T45" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="S45" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="T45" s="0" t="s">
-        <v>450</v>
-      </c>
       <c r="U45" s="0" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="W45" s="11" t="s">
         <v>60</v>
@@ -4668,7 +4662,7 @@
         <v>144</v>
       </c>
       <c r="AC45" s="11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="AD45" s="0" t="n">
         <v>-6.2393418780699</v>
@@ -4679,7 +4673,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>64</v>
@@ -4700,10 +4694,10 @@
         <v>55</v>
       </c>
       <c r="Q46" s="0" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="S46" s="0" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="W46" s="11" t="s">
         <v>60</v>
@@ -4712,7 +4706,7 @@
         <v>5000</v>
       </c>
       <c r="Y46" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Z46" s="0" t="s">
         <v>189</v>
@@ -4724,7 +4718,7 @@
         <v>134</v>
       </c>
       <c r="AC46" s="11" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="AD46" s="0" t="n">
         <v>-6.30418456771596</v>
@@ -4735,7 +4729,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>64</v>
@@ -4756,16 +4750,16 @@
         <v>55</v>
       </c>
       <c r="Q47" s="0" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R47" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="U47" s="0" t="s">
         <v>303</v>
       </c>
       <c r="V47" s="0" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="W47" s="11" t="s">
         <v>306</v>
@@ -4783,10 +4777,10 @@
         <v>307</v>
       </c>
       <c r="AB47" s="11" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="AC47" s="11" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="AD47" s="0" t="n">
         <v>-6.17222481141279</v>
@@ -4797,7 +4791,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>64</v>
@@ -4818,25 +4812,25 @@
         <v>55</v>
       </c>
       <c r="Q48" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="S48" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="R48" s="1" t="s">
+      <c r="W48" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="S48" s="0" t="s">
+      <c r="X48" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="W48" s="11" t="s">
+      <c r="AB48" s="11" t="s">
         <v>467</v>
       </c>
-      <c r="X48" s="9" t="s">
+      <c r="AC48" s="11" t="s">
         <v>468</v>
-      </c>
-      <c r="AB48" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="AC48" s="11" t="s">
-        <v>470</v>
       </c>
       <c r="AD48" s="0" t="n">
         <v>-6.30034768893479</v>
@@ -4847,7 +4841,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>64</v>
@@ -4868,10 +4862,10 @@
         <v>55</v>
       </c>
       <c r="Q49" s="0" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="W49" s="11" t="s">
         <v>60</v>
@@ -4883,7 +4877,7 @@
         <v>144</v>
       </c>
       <c r="AC49" s="11" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="AD49" s="0" t="n">
         <v>-6.30521410272485</v>
@@ -4894,7 +4888,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>50</v>
@@ -4915,22 +4909,22 @@
         <v>201</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="P50" s="0" t="s">
         <v>39</v>
       </c>
       <c r="Q50" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="S50" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="R50" s="1" t="s">
+      <c r="T50" s="0" t="s">
         <v>478</v>
-      </c>
-      <c r="S50" s="0" t="s">
-        <v>479</v>
-      </c>
-      <c r="T50" s="0" t="s">
-        <v>480</v>
       </c>
       <c r="W50" s="11" t="s">
         <v>60</v>
@@ -4939,10 +4933,10 @@
         <v>0</v>
       </c>
       <c r="AB50" s="11" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="AC50" s="11" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="AD50" s="0" t="n">
         <v>-6.1669512894793</v>
@@ -4953,7 +4947,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>106</v>
@@ -4968,13 +4962,13 @@
         <v>37</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="P51" s="0" t="s">
         <v>39</v>
       </c>
       <c r="Q51" s="0" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="W51" s="11" t="s">
         <v>60</v>
@@ -4983,10 +4977,10 @@
         <v>0</v>
       </c>
       <c r="AB51" s="11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="AC51" s="11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="AD51" s="0" t="n">
         <v>-6.20462964280586</v>
@@ -4997,7 +4991,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>106</v>
@@ -5012,34 +5006,34 @@
         <v>53</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="P52" s="0" t="s">
         <v>131</v>
       </c>
       <c r="Q52" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="S52" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="U52" s="0" t="s">
         <v>490</v>
       </c>
-      <c r="S52" s="0" t="s">
+      <c r="V52" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="W52" s="11" t="s">
         <v>491</v>
       </c>
-      <c r="U52" s="0" t="s">
+      <c r="X52" s="9" t="s">
         <v>492</v>
-      </c>
-      <c r="V52" s="0" t="s">
-        <v>492</v>
-      </c>
-      <c r="W52" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="X52" s="9" t="s">
-        <v>494</v>
       </c>
       <c r="AB52" s="11" t="s">
         <v>355</v>
       </c>
       <c r="AC52" s="11" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="AD52" s="0" t="n">
         <v>-6.23169896306931</v>
@@ -5050,7 +5044,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>64</v>
@@ -5065,13 +5059,13 @@
         <v>53</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="P53" s="0" t="s">
         <v>165</v>
       </c>
       <c r="Q53" s="0" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="W53" s="11" t="s">
         <v>304</v>
@@ -5080,10 +5074,10 @@
         <v>305</v>
       </c>
       <c r="AB53" s="11" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="AC53" s="11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="AD53" s="0" t="n">
         <v>-6.13520026432625</v>
@@ -5094,7 +5088,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>32</v>
@@ -5109,46 +5103,46 @@
         <v>53</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="P54" s="0" t="s">
         <v>165</v>
       </c>
       <c r="Q54" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="R54" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="S54" s="0" t="s">
         <v>503</v>
       </c>
-      <c r="R54" s="1" t="s">
+      <c r="U54" s="0" t="s">
         <v>504</v>
       </c>
-      <c r="S54" s="0" t="s">
+      <c r="V54" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="U54" s="0" t="s">
+      <c r="W54" s="11" t="s">
         <v>506</v>
       </c>
-      <c r="V54" s="0" t="s">
+      <c r="X54" s="9" t="s">
         <v>507</v>
       </c>
-      <c r="W54" s="11" t="s">
-        <v>508</v>
-      </c>
-      <c r="X54" s="9" t="s">
-        <v>509</v>
-      </c>
       <c r="Y54" s="9" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="Z54" s="11" t="s">
         <v>189</v>
       </c>
       <c r="AA54" s="9" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="AB54" s="11" t="s">
         <v>126</v>
       </c>
       <c r="AC54" s="11" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="AD54" s="0" t="n">
         <v>-6.13421820441045</v>
@@ -5159,7 +5153,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>246</v>
@@ -5180,13 +5174,13 @@
         <v>55</v>
       </c>
       <c r="Q55" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="R55" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="S55" s="0" t="s">
         <v>513</v>
-      </c>
-      <c r="R55" s="11" t="s">
-        <v>514</v>
-      </c>
-      <c r="S55" s="0" t="s">
-        <v>515</v>
       </c>
       <c r="W55" s="11" t="s">
         <v>60</v>
@@ -5198,7 +5192,7 @@
         <v>159</v>
       </c>
       <c r="AC55" s="11" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="AD55" s="0" t="n">
         <v>-6.30574271489993</v>
@@ -5209,7 +5203,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>64</v>
@@ -5233,28 +5227,28 @@
         <v>175</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="P56" s="0" t="s">
         <v>39</v>
       </c>
       <c r="Q56" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="S56" s="0" t="s">
         <v>519</v>
       </c>
-      <c r="R56" s="1" t="s">
+      <c r="T56" s="0" t="s">
         <v>520</v>
       </c>
-      <c r="S56" s="0" t="s">
+      <c r="U56" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="V56" s="0" t="s">
         <v>521</v>
-      </c>
-      <c r="T56" s="0" t="s">
-        <v>522</v>
-      </c>
-      <c r="U56" s="0" t="s">
-        <v>522</v>
-      </c>
-      <c r="V56" s="0" t="s">
-        <v>523</v>
       </c>
       <c r="W56" s="11" t="s">
         <v>99</v>
@@ -5275,7 +5269,7 @@
         <v>126</v>
       </c>
       <c r="AC56" s="11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="AD56" s="0" t="n">
         <v>-6.18379952050197</v>
@@ -5286,7 +5280,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>32</v>
@@ -5301,43 +5295,43 @@
         <v>53</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="P57" s="0" t="s">
         <v>165</v>
       </c>
       <c r="Q57" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="R57" s="10" t="s">
+        <v>526</v>
+      </c>
+      <c r="U57" s="0" t="s">
         <v>527</v>
       </c>
-      <c r="R57" s="10" t="s">
+      <c r="V57" s="0" t="s">
         <v>528</v>
       </c>
-      <c r="U57" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="V57" s="0" t="s">
-        <v>530</v>
-      </c>
       <c r="W57" s="11" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="X57" s="9" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="Y57" s="9" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="Z57" s="11" t="s">
         <v>189</v>
       </c>
       <c r="AA57" s="9" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="AB57" s="11" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AC57" s="11" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AD57" s="0" t="n">
         <v>-6.18796452926196</v>
@@ -5348,7 +5342,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>64</v>
@@ -5369,13 +5363,13 @@
         <v>55</v>
       </c>
       <c r="Q58" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="S58" s="0" t="s">
         <v>534</v>
-      </c>
-      <c r="R58" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="S58" s="0" t="s">
-        <v>536</v>
       </c>
       <c r="W58" s="11" t="s">
         <v>60</v>
@@ -5384,10 +5378,10 @@
         <v>5000</v>
       </c>
       <c r="AB58" s="11" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AC58" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="AD58" s="0" t="n">
         <v>-6.30331509392487</v>
@@ -5398,7 +5392,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>64</v>
@@ -5413,25 +5407,25 @@
         <v>53</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="P59" s="0" t="s">
         <v>165</v>
       </c>
       <c r="Q59" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="S59" s="0" t="s">
         <v>541</v>
       </c>
-      <c r="R59" s="1" t="s">
+      <c r="U59" s="0" t="s">
         <v>542</v>
       </c>
-      <c r="S59" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="U59" s="0" t="s">
-        <v>544</v>
-      </c>
       <c r="V59" s="0" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="W59" s="11" t="s">
         <v>60</v>
@@ -5440,10 +5434,10 @@
         <v>0</v>
       </c>
       <c r="AB59" s="11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="AC59" s="11" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="AD59" s="0" t="n">
         <v>-6.16770993445603</v>
@@ -5454,7 +5448,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>298</v>
@@ -5475,28 +5469,28 @@
         <v>55</v>
       </c>
       <c r="Q60" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="R60" s="10" t="s">
+        <v>547</v>
+      </c>
+      <c r="S60" s="11" t="s">
         <v>548</v>
       </c>
-      <c r="R60" s="10" t="s">
+      <c r="U60" s="0" t="s">
         <v>549</v>
       </c>
-      <c r="S60" s="11" t="s">
+      <c r="W60" s="11" t="s">
         <v>550</v>
       </c>
-      <c r="U60" s="0" t="s">
+      <c r="X60" s="9" t="s">
         <v>551</v>
-      </c>
-      <c r="W60" s="11" t="s">
-        <v>552</v>
-      </c>
-      <c r="X60" s="9" t="s">
-        <v>553</v>
       </c>
       <c r="AB60" s="11" t="s">
         <v>144</v>
       </c>
       <c r="AC60" s="11" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="AD60" s="0" t="n">
         <v>-6.30491375819847</v>
@@ -5507,7 +5501,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>32</v>
@@ -5522,31 +5516,31 @@
         <v>53</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="P61" s="0" t="s">
         <v>165</v>
       </c>
       <c r="Q61" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="U61" s="0" t="s">
         <v>557</v>
       </c>
-      <c r="R61" s="1" t="s">
+      <c r="W61" s="11" t="s">
         <v>558</v>
       </c>
-      <c r="U61" s="0" t="s">
+      <c r="X61" s="9" t="s">
         <v>559</v>
-      </c>
-      <c r="W61" s="11" t="s">
-        <v>560</v>
-      </c>
-      <c r="X61" s="9" t="s">
-        <v>561</v>
       </c>
       <c r="AB61" s="11" t="s">
         <v>134</v>
       </c>
       <c r="AC61" s="11" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="AD61" s="0" t="n">
         <v>-6.13490616619183</v>
@@ -5557,7 +5551,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>137</v>
@@ -5596,22 +5590,22 @@
         <v>55</v>
       </c>
       <c r="Q62" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="R62" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="S62" s="0" t="s">
         <v>564</v>
       </c>
-      <c r="R62" s="10" t="s">
+      <c r="T62" s="0" t="s">
         <v>565</v>
       </c>
-      <c r="S62" s="0" t="s">
+      <c r="U62" s="0" t="s">
         <v>566</v>
       </c>
-      <c r="T62" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="U62" s="0" t="s">
-        <v>568</v>
-      </c>
       <c r="V62" s="0" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="W62" s="11" t="s">
         <v>60</v>
@@ -5623,7 +5617,7 @@
         <v>144</v>
       </c>
       <c r="AC62" s="11" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="AD62" s="0" t="n">
         <v>-6.30221876193348</v>

</xml_diff>

<commit_message>
add input form ticket_price
</commit_message>
<xml_diff>
--- a/datasets/raw_dataset.xlsx
+++ b/datasets/raw_dataset.xlsx
@@ -308,7 +308,7 @@
     <t xml:space="preserve">07:00</t>
   </si>
   <si>
-    <t xml:space="preserve">00:00</t>
+    <t xml:space="preserve">24:00</t>
   </si>
   <si>
     <t xml:space="preserve">Jl. Tugu Monas, Gambir, Jakarta Pusat, DKI Jakarta</t>
@@ -2247,19 +2247,19 @@
   <dimension ref="A1:AE62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="AB1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="X32" activeCellId="0" sqref="X32"/>
+      <selection pane="topRight" activeCell="AB18" activeCellId="0" sqref="AB18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="54.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="37.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="19.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="44.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="23.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="14.99"/>
@@ -5931,8 +5931,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5951,7 +5951,7 @@
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -6261,10 +6261,10 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
able to query knowledge graph
</commit_message>
<xml_diff>
--- a/datasets/raw_dataset.xlsx
+++ b/datasets/raw_dataset.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="572">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -1737,177 +1736,6 @@
   </si>
   <si>
     <t xml:space="preserve">46.2, 11.9, 24.1, 24, 5.8, 16.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRM Translation = E53 Place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P87 is identified by (identifies) E41 Place Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2 has type (is type of) E55 Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P89 falls within (contains) E53 Place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P87 is identified by (identifies) E45 Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P87 is identified by (identifies) E47 Spatial Coordinates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1 is identified by (identifies) E51 Contact Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://…..com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facebook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instagram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twitter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schedule (category)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schedule 1, Schedule 2, Schedule 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schedule value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senin, Selasa, … , Minggu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2 has type (is type of) E55 Type P45 consists of (is incorporated in) E49 Time Appellation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schedule Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pameran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2 has type (is type of) E55 Type P45 consists of (is incorporated in) E49 Time Appellation P1 is identified by (identifies) E41 Appellation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2 has type (is type of) E55 Type P45 consists of (is incorporated in) E49 Time Appellation P81 ongoing throughout E52 Time-Span</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticket Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticket 1, Ticket 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticket types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wisatawan Mancanegara, … , Pelajar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2 has type (is type of) E55 Type P2 has type (is type of) E55 Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticket Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2 has type (is type of) E55 Type P2 has type (is type of) E55 Type P1 is identified by (identifies) E41 Appellation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticket Price</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">P2 has type (is type of) E55 Type P2 has type (is type of) E55 Type P90 has value </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">E60 Number</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Transportation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bandara Halim, … , Terminal Senen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2 has type E55 Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transportation Distance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2 has type E55 Type P90 has value E60 Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Missing Properties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject to Change</t>
   </si>
 </sst>
 </file>
@@ -1921,7 +1749,7 @@
     <numFmt numFmtId="167" formatCode="hh:mm"/>
     <numFmt numFmtId="168" formatCode="[$-421]hh:mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1952,64 +1780,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4C7DC"/>
-        <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00A933"/>
-        <bgColor rgb="FF008000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -2041,7 +1826,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2090,82 +1875,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2192,7 +1901,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -2227,7 +1936,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -2249,10 +1958,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="AB1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AB18" activeCellId="0" sqref="AB18"/>
+      <selection pane="topRight" activeCell="AB9" activeCellId="0" sqref="AB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="54.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.86"/>
@@ -5938,333 +5647,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G30"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.09"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>572</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>573</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>575</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
-        <v>577</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
-        <v>579</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
-        <v>581</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>583</v>
-      </c>
-      <c r="B6" s="19" t="n">
-        <v>-6.14695017338058</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
-        <v>585</v>
-      </c>
-      <c r="B7" s="19" t="n">
-        <v>106.840289461744</v>
-      </c>
-      <c r="C7" s="20"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
-        <v>586</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
-        <v>588</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="21"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
-        <v>589</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>590</v>
-      </c>
-      <c r="C10" s="21"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
-        <v>591</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="21"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
-        <v>592</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="21"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
-        <v>593</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="21"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
-        <v>594</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>595</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
-        <v>596</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>597</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
-        <v>599</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>600</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
-        <v>602</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
-        <v>604</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="20"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="24"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
-        <v>605</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>606</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
-        <v>607</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>608</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
-        <v>610</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
-        <v>612</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="26"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16" t="s">
-        <v>614</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>615</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="16" t="s">
-        <v>617</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="27"/>
-      <c r="F28" s="28" t="s">
-        <v>619</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="29"/>
-      <c r="F29" s="28" t="s">
-        <v>619</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="30"/>
-      <c r="F30" s="28" t="s">
-        <v>619</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>622</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="C18:C19"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>